<commit_message>
better test data, clean up docstrings
</commit_message>
<xml_diff>
--- a/data/sessions.xlsx
+++ b/data/sessions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcdermott/code/github/appt-scheduling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcdermott/code/github/caseload-scheduling/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508CFAA8-FA4E-BF42-AA89-DFB02A87DC65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC6FD4C-FB47-1D49-8054-518FF6E3C9EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14600" yWindow="920" windowWidth="27640" windowHeight="16940" xr2:uid="{94FC90EC-69F7-D84B-8B83-2419A711D246}"/>
+    <workbookView xWindow="8260" yWindow="12020" windowWidth="27640" windowHeight="16940" xr2:uid="{94FC90EC-69F7-D84B-8B83-2419A711D246}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -409,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC99B3EC-4F08-A649-BD32-48DF4858DBCD}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -456,15 +456,92 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.50694444444444442</v>
-      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>